<commit_message>
CNY 3M Shibor Curve first version
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CNY_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CNY_MainChecks.xlsx
@@ -16,11 +16,11 @@
     <definedName name="AllTriggers">MainChecks!$I$5:$I$5</definedName>
     <definedName name="Currency">MainChecks!$B$1</definedName>
     <definedName name="EvaluationDate">MainChecks!$C$3</definedName>
-    <definedName name="FirstIndex">MainChecks!$B$11</definedName>
+    <definedName name="FirstIndex">MainChecks!$B$8</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!$I$5</definedName>
-    <definedName name="SecondIMMDate">MainChecks!$C$12</definedName>
+    <definedName name="SecondIMMDate">MainChecks!$C$9</definedName>
     <definedName name="Trigger">MainChecks!$I$2</definedName>
-    <definedName name="Yesterday">MainChecks!$C$9</definedName>
+    <definedName name="Yesterday">MainChecks!$C$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -578,7 +578,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -689,9 +689,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="170" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -790,9 +787,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Not Signed In</v>
+        <v>Updated at 12:12:22</v>
         <stp/>
-        <stp>{CE79C657-B64A-474F-A89C-93F21BC31D49}</stp>
+        <stp>{FFE4517E-B3AC-4509-BA82-8F1EABE040B8}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -900,31 +897,17 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="General Settings"/>
-      <sheetName val="Libor"/>
-      <sheetName val="LiborSwapIsdaFixAm"/>
-      <sheetName val="LiborSwapForBasisCalc"/>
-      <sheetName val="LiborSwapIsdaFixPm"/>
-      <sheetName val="BasisSwap1MxM"/>
-      <sheetName val="BasisSwap3M6M"/>
-      <sheetName val="BasisSwapxM12M"/>
+      <sheetName val="Shibor"/>
+      <sheetName val="RepoRates"/>
       <sheetName val="Deposits"/>
+      <sheetName val="OIS"/>
       <sheetName val="FRA"/>
       <sheetName val="Futures1M"/>
       <sheetName val="Futures3M"/>
-      <sheetName val="ImmFra6M "/>
       <sheetName val="FuturesHWConvAdj"/>
-      <sheetName val="OIS"/>
       <sheetName val="Swaps1M"/>
-      <sheetName val="SwapsIMMDated"/>
       <sheetName val="Swap3M"/>
-      <sheetName val="Swap6M"/>
-      <sheetName val="ON"/>
-      <sheetName val="1M (2)"/>
-      <sheetName val="3M (2)"/>
-      <sheetName val="FwdEONIAOIS"/>
-      <sheetName val="SFIX3"/>
-      <sheetName val="IB365"/>
-      <sheetName val="IBOR"/>
+      <sheetName val="Swap7DRepo"/>
     </sheetNames>
     <definedNames>
       <definedName name="TriggerCounter" refersTo="='General Settings'!$D$7"/>
@@ -933,164 +916,78 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>1</v>
+            <v>3</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="D7">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="2">
         <row r="7">
-          <cell r="D7" t="str">
-            <v>3M</v>
+          <cell r="D7">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="7">
           <cell r="D7" t="str">
-            <v>Fwd Curve</v>
+            <v>CNY2WD_Quote#0000</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
         <row r="7">
           <cell r="D7" t="str">
-            <v>3M</v>
+            <v>3W</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="5">
         <row r="7">
           <cell r="D7" t="str">
-            <v>1L</v>
+            <v>CNY3x6F_Quote</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="6">
         <row r="7">
           <cell r="D7" t="str">
-            <v>3L</v>
+            <v>Q4</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="7">
         <row r="7">
           <cell r="D7" t="str">
-            <v>3L</v>
+            <v>Q4</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="8">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USDSND_Quote#0000</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="8"/>
       <sheetData sheetId="9">
         <row r="7">
           <cell r="D7" t="str">
-            <v>USD1x4F_Quote</v>
+            <v>X1S</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="10">
         <row r="7">
           <cell r="D7" t="str">
-            <v>N4</v>
+            <v>3AB</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="11">
         <row r="7">
           <cell r="D7" t="str">
-            <v>N4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>V4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3W</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>X1S</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
-        <row r="7">
-          <cell r="D7">
-            <v>12</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="17">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="18">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="21">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="22">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>2X</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="23">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-4Y=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="24">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-SWD=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="25">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-SWD=</v>
+            <v>6AB</v>
           </cell>
         </row>
       </sheetData>
@@ -1389,7 +1286,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W59"/>
+  <dimension ref="A1:W58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -1397,8 +1294,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="5" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" bestFit="1" customWidth="1"/>
@@ -1459,9 +1356,7 @@
       <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="39">
-        <v>41806.543877314813</v>
-      </c>
+      <c r="I2" s="39"/>
       <c r="J2" s="13"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1483,9 +1378,9 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>CNYSTD</v>
       </c>
-      <c r="C3" s="48" t="e">
+      <c r="C3" s="48">
         <f>_xll.qlCalendarAdjust(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
-        <v>#VALUE!</v>
+        <v>41810</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="e">
@@ -1494,7 +1389,7 @@
       </c>
       <c r="F3" s="18" t="str">
         <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v/>
+        <v>qlYieldTSDiscount - ObjectHandler error: attempt to retrieve object with unknown ID 'CNYSTD'</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="46" t="s">
@@ -1502,7 +1397,7 @@
       </c>
       <c r="I3" s="45" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Not Signed In</v>
+        <v>Updated at 12:12:22</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="4"/>
@@ -1522,12 +1417,12 @@
     <row r="4" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="15" t="str">
-        <f>UPPER(Currency)&amp;"ON"</f>
-        <v>CNYON</v>
-      </c>
-      <c r="C4" s="40" t="e">
+        <f>UPPER(Currency)&amp;"7DREPO"</f>
+        <v>CNY7DREPO</v>
+      </c>
+      <c r="C4" s="40">
         <f>EvaluationDate</f>
-        <v>#VALUE!</v>
+        <v>41810</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17" t="e">
@@ -1536,14 +1431,14 @@
       </c>
       <c r="F4" s="18" t="str">
         <f ca="1">IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(E4))</f>
-        <v/>
+        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="47" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="44">
-        <v>124.71875</v>
+        <v>124.3125</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="4"/>
@@ -1563,12 +1458,12 @@
     <row r="5" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="15" t="str">
-        <f>UPPER(Currency)&amp;"1M"</f>
-        <v>CNY1M</v>
-      </c>
-      <c r="C5" s="40" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D","Following")</f>
-        <v>#VALUE!</v>
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>CNY3M</v>
+      </c>
+      <c r="C5" s="40">
+        <f>C4</f>
+        <v>41810</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="17" t="e">
@@ -1577,7 +1472,7 @@
       </c>
       <c r="F5" s="18" t="str">
         <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
-        <v>qlInterestRateIndexFixingDays - ObjectHandler error: attempt to retrieve object with unknown ID 'CnyLibor3M'</v>
+        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="19" t="s">
@@ -1585,7 +1480,7 @@
       </c>
       <c r="I5" s="20">
         <f>[1]!TriggerCounter</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="4"/>
@@ -1604,22 +1499,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="B6" s="15" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>CNY3M</v>
-      </c>
-      <c r="C6" s="40" t="e">
-        <f>C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17" t="e">
-        <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
+      <c r="B6" s="23"/>
+      <c r="C6" s="41">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
+        <v>41808</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C6)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F6" s="18" t="str">
+      <c r="F6" s="14" t="str">
         <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v/>
+        <v>qlIndexFixing - Missing Shibor3M Actual/360 fixing for June 18th, 2014</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="19" t="s">
@@ -1627,7 +1519,7 @@
       </c>
       <c r="I6" s="20">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>735</v>
+        <v>256</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="4"/>
@@ -1646,21 +1538,18 @@
     </row>
     <row r="7" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="15" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>CNY6M</v>
-      </c>
-      <c r="C7" s="40" t="e">
-        <f>C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17" t="e">
-        <f>_xll.qlYieldTSDiscount(B7,C7,,Trigger)</f>
-        <v>#NUM!</v>
+      <c r="B7" s="26"/>
+      <c r="C7" s="42">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
+        <v>41809</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="28">
+        <f>_xll.qlIndexFixing(FirstIndex,C7)</f>
+        <v>4.7691999999999998E-2</v>
       </c>
       <c r="F7" s="18" t="str">
-        <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
+        <f>IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
         <v/>
       </c>
       <c r="G7" s="11"/>
@@ -1685,23 +1574,23 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="15" t="str">
-        <f>UPPER(Currency)&amp;"1Y"</f>
-        <v>CNY1Y</v>
-      </c>
-      <c r="C8" s="40" t="e">
-        <f>C7</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="17" t="e">
-        <f>_xll.qlYieldTSDiscount(B8,C8,,Trigger)</f>
-        <v>#NUM!</v>
+      <c r="B8" s="26" t="str">
+        <f>PROPER(Currency)&amp;"Shibor3M"</f>
+        <v>CnyShibor3M</v>
+      </c>
+      <c r="C8" s="42">
+        <f>EvaluationDate</f>
+        <v>41810</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28">
+        <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
+        <v>4.7751000000000002E-2</v>
       </c>
       <c r="F8" s="18" t="str">
-        <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
+        <f>IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
         <v/>
       </c>
       <c r="G8" s="11"/>
@@ -1727,23 +1616,23 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="41" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
+      <c r="B9" s="29"/>
+      <c r="C9" s="43">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>41990</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C9,TRUE)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="14" t="str">
+      <c r="F9" s="32" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixingCalendar - ObjectHandler error: attempt to retrieve object with unknown ID 'CnyLibor3M'</v>
-      </c>
-      <c r="G9" s="11"/>
+        <v>qlIndexFixing - null term structure set to this instance of Shibor3M Actual/360</v>
+      </c>
+      <c r="G9" s="50"/>
       <c r="H9" s="21" t="s">
         <v>9</v>
       </c>
@@ -1768,21 +1657,12 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="42" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="28" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" s="18" t="str">
-        <f ca="1">IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
-        <v>qlIndexFixingCalendar - ObjectHandler error: attempt to retrieve object with unknown ID 'CnyLibor3M'</v>
-      </c>
-      <c r="G10" s="11"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
       <c r="H10" s="21" t="s">
         <v>10</v>
       </c>
@@ -1807,24 +1687,12 @@
     </row>
     <row r="11" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="26" t="str">
-        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor3M"</f>
-        <v>CnyLibor3M</v>
-      </c>
-      <c r="C11" s="42" t="e">
-        <f>EvaluationDate</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F11" s="18" t="str">
-        <f ca="1">IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
-        <v/>
-      </c>
-      <c r="G11" s="11"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
       <c r="H11" s="33" t="s">
         <v>11</v>
       </c>
@@ -1848,25 +1716,16 @@
       <c r="W11" s="4"/>
     </row>
     <row r="12" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="43" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C12,TRUE)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F12" s="32" t="str">
-        <f ca="1">IF(ISERROR(C12),_xll.ohRangeRetrieveError(C12),_xll.ohRangeRetrieveError(E12))</f>
-        <v>qlInterestRateIndexFixingDays - ObjectHandler error: attempt to retrieve object with unknown ID 'CnyLibor3M'</v>
-      </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="13"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -1881,17 +1740,17 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
     </row>
-    <row r="13" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -2888,9 +2747,6 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -2908,12 +2764,6 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
@@ -2929,7 +2779,6 @@
       <c r="W54" s="4"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
@@ -2988,21 +2837,6 @@
       <c r="U58" s="4"/>
       <c r="V58" s="4"/>
       <c r="W58" s="4"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3019,7 +2853,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -3039,12 +2873,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -3064,7 +2898,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>